<commit_message>
Update before formatting windows
</commit_message>
<xml_diff>
--- a/releases/cw1.0 (improved, helmet lid)/bom.xlsx
+++ b/releases/cw1.0 (improved, helmet lid)/bom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruben\Documents\GitHub\cyberwheel\releases\cw1.0 (improved, helmet lid)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B07A33A9-F232-478D-9A21-DFF647B25A1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E52FBE8D-482D-40DA-AE2A-05E9DE9D2489}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D88DFB00-99BE-4A0F-B4EA-8B30B61E7E0B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>Componente</t>
   </si>
@@ -80,16 +80,37 @@
     <t>Separadores de plástico</t>
   </si>
   <si>
-    <t>TOTAL:</t>
-  </si>
-  <si>
     <t>Coste mano de obra (15€/h * 20h)</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Coste</t>
+  </si>
+  <si>
+    <t>Motor+Rim</t>
+  </si>
+  <si>
+    <t>Tyre</t>
+  </si>
+  <si>
+    <t>Mano de obra ensamblaje (30h * 15€/h)</t>
+  </si>
+  <si>
+    <t>Ignorando mano de obra, con batería fabricada:</t>
+  </si>
+  <si>
+    <t>Tapa exterior</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0\ [$€-1];[Red]\-#,##0\ [$€-1]"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -119,8 +140,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -477,21 +499,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F60FE30-6133-413C-B78E-0FBAE8FABF31}">
-  <dimension ref="B2:I14"/>
+  <dimension ref="B2:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="41.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
       <c r="H2" t="s">
         <v>6</v>
       </c>
@@ -546,59 +571,100 @@
         <v>700</v>
       </c>
       <c r="H6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="I6">
+      <c r="C7">
         <v>52</v>
       </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8">
+        <v>200</v>
+      </c>
+      <c r="H8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9">
+        <v>50</v>
+      </c>
+      <c r="H9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9">
         <v>10</v>
       </c>
-      <c r="I7">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H8" t="s">
-        <v>11</v>
-      </c>
-      <c r="I8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H9" t="s">
-        <v>12</v>
-      </c>
-      <c r="I9">
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10">
+        <v>450</v>
+      </c>
+      <c r="H10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H10" t="s">
-        <v>13</v>
-      </c>
-      <c r="I10">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H11" t="s">
-        <v>15</v>
-      </c>
-      <c r="I11">
-        <v>300</v>
+      <c r="C13">
+        <f>SUM(C4:C12)</f>
+        <v>1912</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I14">
         <f>SUM(I4:I13)</f>
-        <v>580</v>
+        <v>528</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="1">
+        <v>990</v>
       </c>
     </row>
   </sheetData>

</xml_diff>